<commit_message>
Updates with fixed graphs
</commit_message>
<xml_diff>
--- a/Comment_Data.xlsx
+++ b/Comment_Data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\python\IA626-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B51CF0F-F74C-4513-9A42-3FAAF521952B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F167EB27-461A-4C87-B013-55FFFF8946EA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -356,7 +356,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -930,8 +930,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Removed Comments Over Time</a:t>
+              <a:t>Number</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of Removed Comments Over Time</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -968,7 +973,7 @@
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="stacked"/>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1246,7 +1251,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-CBDF-4457-B34E-3E547FD5534D}"/>
+              <c16:uniqueId val="{00000001-846B-40AB-B293-DEC6C9DDCAED}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1254,7 +1259,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>COVID19</c:v>
+            <c:v>COVID119</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1526,7 +1531,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-CBDF-4457-B34E-3E547FD5534D}"/>
+              <c16:uniqueId val="{00000003-846B-40AB-B293-DEC6C9DDCAED}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1540,73 +1545,18 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="106196927"/>
-        <c:axId val="113020319"/>
+        <c:axId val="1881930591"/>
+        <c:axId val="1731437263"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="106196927"/>
+        <c:axId val="1881930591"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Dates</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="m/d/yyyy\ h:mm" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1642,14 +1592,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113020319"/>
+        <c:crossAx val="1731437263"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="113020319"/>
+        <c:axId val="1731437263"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1690,8 +1640,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Removed Comments</a:t>
+                  <a:t>Number</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Removed Comments</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1755,7 +1710,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="106196927"/>
+        <c:crossAx val="1881930591"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1799,15 +1754,9 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4197,11 +4146,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5572,11 +5521,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>